<commit_message>
corretto errore test execution
</commit_message>
<xml_diff>
--- a/dmn/test/new_UserQualifications-MasterGlobalDef304_test.xlsx
+++ b/dmn/test/new_UserQualifications-MasterGlobalDef304_test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauriziocaronni/Projects/DmnEngine/dmn/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD5B8E0-6EC6-3048-856E-4CC35E1FCE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F898E04-E362-C44B-A29F-058A95850182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4480" yWindow="500" windowWidth="31360" windowHeight="20200" xr2:uid="{E34855F7-CB3F-8345-982A-7C4A7DDB4B0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -588,9 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE88A2E-37D4-F745-8E0C-CF21D2FAD894}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -943,4 +942,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A57376-5D97-1245-B0A7-A69FA97A11B4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>